<commit_message>
tested for other values, dropped the ones that for too long
</commit_message>
<xml_diff>
--- a/PracaNaLekcji4/wyniki.xlsx
+++ b/PracaNaLekcji4/wyniki.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\SCI_INF\PracaNaLekcji4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41B5F14-344D-4A9F-992D-C07CE46E260B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A857975-EEF7-4C0F-8795-EB68AB3EAF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8520" yWindow="1905" windowWidth="28800" windowHeight="11385" xr2:uid="{370D3B2A-A3FF-48E4-9A7E-75BC805C353B}"/>
+    <workbookView xWindow="8865" yWindow="2250" windowWidth="28800" windowHeight="12660" xr2:uid="{370D3B2A-A3FF-48E4-9A7E-75BC805C353B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>sortowanie</t>
   </si>
@@ -67,6 +67,24 @@
   </si>
   <si>
     <t>std</t>
+  </si>
+  <si>
+    <t>trzeba użyć tail call optimisation, bez tego jest stack overflow</t>
+  </si>
+  <si>
+    <t>dla 1000 elementów najlepszy jest std/introsort jest 165 razy szybszy od bubble sorta</t>
+  </si>
+  <si>
+    <t>dla 100000 elementów najlepszy jest std/introsort jest 12701 razy szybszy od bubble sorta</t>
+  </si>
+  <si>
+    <t>dla 10000 elementów najlepszy jest std/introsort jest 1466 razy szybszy od bubble sorta</t>
+  </si>
+  <si>
+    <t>program utyka i nagle zaczyna zajmować ogromne ilości ramu</t>
+  </si>
+  <si>
+    <t>program nigdy nie dochodzi do tego momentu</t>
   </si>
 </sst>
 </file>
@@ -74,7 +92,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0000000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000000000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -99,9 +117,124 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -111,9 +244,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,358 +576,634 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1024B2B5-C0DD-444C-A7B6-8EB60706783E}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="56.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="81.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>100</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>3.39E-4</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>6.4899999999999995E-4</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>1.2149999999999999E-3</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="5">
         <f>AVERAGE(C2:E2)</f>
         <v>7.3433333333333337E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>100</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>1.4E-5</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>1.4E-5</v>
       </c>
-      <c r="F3" s="1">
-        <f t="shared" ref="F3:F16" si="0">AVERAGE(C3:E3)</f>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F11" si="0">AVERAGE(C3:E3)</f>
         <v>1.2666666666666667E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>100</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>6.3999999999999997E-5</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>8.1000000000000004E-5</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>1.12E-4</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="3">
         <f t="shared" si="0"/>
         <v>8.5666666666666671E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>100</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>1.3899999999999999E-4</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>2.7900000000000001E-4</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>4.8899999999999996E-4</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="3">
         <f t="shared" si="0"/>
         <v>3.0233333333333333E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>100</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>3.6000000000000001E-5</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>6.8999999999999997E-5</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="3">
         <f>AVERAGE(C12:E12)</f>
         <v>4.5399999999999998E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>1000</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>3.8970999999999999E-2</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>6.9210999999999995E-2</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>0.117329</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>7.5170333333333339E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="G8" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>1000</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>1.2E-4</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>1.134E-3</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>1.0859999999999999E-3</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>7.7999999999999999E-4</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>1000</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>6.698E-3</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>7.6540000000000002E-3</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>1.1657000000000001E-2</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="3">
         <f t="shared" si="0"/>
         <v>8.6696666666666675E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>1000</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>1.1795999999999999E-2</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>2.6195E-2</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>4.6577E-2</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="3">
         <f t="shared" si="0"/>
         <v>2.8189333333333334E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>1000</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>3.2899999999999997E-4</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>4.6500000000000003E-4</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>5.6800000000000004E-4</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="3">
         <f>AVERAGE(C12:E12)</f>
         <v>4.5399999999999998E-4</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="G12" s="14"/>
+      <c r="H12">
+        <f>F8/F12</f>
+        <v>165.57342143906024</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>10000</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>3.8206920000000002</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>6.9926519999999996</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>11.878026999999999</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="3">
         <f>AVERAGE(C14:E14)</f>
         <v>7.5637903333333334</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="G14" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>10000</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>1.3829999999999999E-3</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>4.6135000000000002E-2</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>4.4467E-2</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="3">
         <f>AVERAGE(C15:E15)</f>
         <v>3.066166666666667E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>10000</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>0.613236</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>0.76530100000000001</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>1.085501</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="3">
         <f>AVERAGE(C16:E16)</f>
         <v>0.82134600000000013</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>10000</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>1.146973</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>2.5931320000000002</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>4.6035139999999997</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="3">
         <f>AVERAGE(C17:E17)</f>
         <v>2.7812063333333334</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>10000</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>3.7780000000000001E-3</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>5.1349999999999998E-3</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>6.5579999999999996E-3</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="10">
         <f>AVERAGE(C18:E18)</f>
         <v>5.1570000000000001E-3</v>
       </c>
+      <c r="G18" s="14"/>
+      <c r="H18">
+        <f>F14/F18</f>
+        <v>1466.7035744295779</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2">
+        <v>100000</v>
+      </c>
+      <c r="C20" s="2">
+        <v>384.268081</v>
+      </c>
+      <c r="D20" s="2">
+        <v>715.57319900000005</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1192.717535</v>
+      </c>
+      <c r="F20" s="5">
+        <f t="shared" ref="F19:F41" si="1">AVERAGE(C20:E20)</f>
+        <v>764.18627166666681</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="2">
+        <v>100000</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1.5328E-2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.81128500000000003</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.815612</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="1"/>
+        <v>0.54740833333333339</v>
+      </c>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="2">
+        <v>100000</v>
+      </c>
+      <c r="C22" s="2">
+        <v>61.726717000000001</v>
+      </c>
+      <c r="D22" s="2">
+        <v>77.345427999999998</v>
+      </c>
+      <c r="E22" s="2">
+        <v>108.010671</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="1"/>
+        <v>82.360938666666669</v>
+      </c>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="2">
+        <v>100000</v>
+      </c>
+      <c r="C23" s="2">
+        <v>115.150795</v>
+      </c>
+      <c r="D23" s="2">
+        <v>259.60154599999998</v>
+      </c>
+      <c r="E23" s="2">
+        <v>460.86706299999997</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="1"/>
+        <v>278.53980133333334</v>
+      </c>
+      <c r="G23" s="14"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="2">
+        <v>100000</v>
+      </c>
+      <c r="C24" s="2">
+        <v>4.3984000000000002E-2</v>
+      </c>
+      <c r="D24" s="2">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="E24" s="2">
+        <v>7.7813999999999994E-2</v>
+      </c>
+      <c r="F24" s="10">
+        <f t="shared" si="1"/>
+        <v>6.0165999999999997E-2</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24">
+        <f>F20/F24</f>
+        <v>12701.297604405592</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="C26" s="2">
+        <v>4.9787699999999997E-2</v>
+      </c>
+      <c r="D26" s="2">
+        <v>6.1448700000000002E-2</v>
+      </c>
+      <c r="E26" s="2">
+        <v>7.7999200000000005E-2</v>
+      </c>
+      <c r="F26" s="5">
+        <f t="shared" si="1"/>
+        <v>6.3078533333333339E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1.7790500000000001E-2</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1.7960499999999999</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1.77911</v>
+      </c>
+      <c r="F27" s="10">
+        <f t="shared" si="1"/>
+        <v>1.1976501666666666</v>
+      </c>
+      <c r="G27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F28" s="13"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.83270200000000005</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.78351199999999999</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.94780500000000001</v>
+      </c>
+      <c r="F29" s="5">
+        <f t="shared" ref="F29:F30" si="2">AVERAGE(C29:E29)</f>
+        <v>0.85467300000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.55320599999999998</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="10">
+        <f t="shared" si="2"/>
+        <v>0.55320599999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F31" s="11"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="11"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="11"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="11"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="11"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="11"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="11"/>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="11"/>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="11"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="G8:G12"/>
+    <mergeCell ref="G14:G18"/>
+    <mergeCell ref="G20:G24"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>